<commit_message>
Updated the supplement PDUFA fees based on year
</commit_message>
<xml_diff>
--- a/PDUFAFees.xlsx
+++ b/PDUFAFees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbff180949efc752/Documents/UMGC/Summit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_F25DC773A252ABDACC10480DF9186DE25ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19FDF3A9-E441-49F2-A77B-B614D28714E6}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="11_F25DC773A252ABDACC10480DF9186DE25ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5DCB158-8768-41A6-BCC3-CF8ADB5573A1}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="3615" windowWidth="17010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3615" windowWidth="17010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Year</t>
   </si>
   <si>
     <t>Fees</t>
+  </si>
+  <si>
+    <t>SupplementFees</t>
   </si>
 </sst>
 </file>
@@ -111,12 +114,17 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{87878A53-A9EC-40C9-A8F5-004508776FEC}" name="Table1" displayName="Table1" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33" xr:uid="{87878A53-A9EC-40C9-A8F5-004508776FEC}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{87878A53-A9EC-40C9-A8F5-004508776FEC}" name="Table1" displayName="Table1" ref="A1:C33" totalsRowShown="0">
+  <autoFilter ref="A1:C33" xr:uid="{87878A53-A9EC-40C9-A8F5-004508776FEC}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AA05E70C-9E9A-45EA-B815-5B857E4DEB1B}" name="Year"/>
     <tableColumn id="2" xr3:uid="{0EC9C6B0-EFDC-45B3-877C-899CB67E86CD}" name="Fees" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{EDAA19FD-2C54-484E-9694-40068EB27F07}" name="SupplementFees" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -385,279 +393,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H10"/>
+      <selection activeCell="I25" sqref="I24:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1993</v>
       </c>
       <c r="B2" s="4">
         <v>100000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1994</v>
       </c>
       <c r="B3" s="4">
         <v>150000</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="1">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1995</v>
       </c>
       <c r="B4" s="4">
         <v>208000</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="3">
+        <v>104000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>1996</v>
       </c>
       <c r="B5" s="2">
         <v>204000</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="3">
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>1997</v>
       </c>
       <c r="B6" s="2">
         <v>205000</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="3">
+        <v>102500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>1998</v>
       </c>
       <c r="B7" s="1">
         <v>256846</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="1">
+        <v>128423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>1999</v>
       </c>
       <c r="B8" s="1">
         <v>272282</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="1">
+        <v>136141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2000</v>
       </c>
       <c r="B9" s="1">
         <v>256338</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="3">
+        <v>142870</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2001</v>
       </c>
       <c r="B10" s="1">
         <v>267606</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="1">
+        <v>133803</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>2002</v>
       </c>
       <c r="B11" s="1">
         <v>258451</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="1">
+        <v>129226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2003</v>
       </c>
       <c r="B12" s="1">
         <v>533400</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="1">
+        <v>266700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2004</v>
       </c>
       <c r="B13" s="1">
         <v>573500</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="1">
+        <v>286750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>2005</v>
       </c>
       <c r="B14" s="1">
         <v>672000</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="1">
+        <v>262200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>2006</v>
       </c>
       <c r="B15" s="1">
         <v>767400</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="1">
+        <v>383700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>2007</v>
       </c>
       <c r="B16" s="1">
         <v>896200</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="1">
+        <v>448100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2008</v>
       </c>
       <c r="B17" s="1">
         <v>1178000</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="1">
+        <v>589000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>2009</v>
       </c>
       <c r="B18" s="1">
         <v>1247200</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="1">
+        <v>623600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>2010</v>
       </c>
       <c r="B19" s="1">
         <v>1405500</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="1">
+        <v>702750</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>2011</v>
       </c>
       <c r="B20" s="3">
         <v>1542000</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="1">
+        <v>771000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>2012</v>
       </c>
       <c r="B21" s="1">
         <v>1841500</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="1">
+        <v>920750</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>2013</v>
       </c>
       <c r="B22" s="1">
         <v>1958800</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="1">
+        <v>979400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>2014</v>
       </c>
       <c r="B23" s="1">
         <v>2169100</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="1">
+        <v>1084550</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>2015</v>
       </c>
       <c r="B24" s="1">
         <v>2335200</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="1">
+        <v>1167600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>2016</v>
       </c>
       <c r="B25" s="1">
         <v>2374200</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="1">
+        <v>1187100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>2017</v>
       </c>
       <c r="B26" s="1">
         <v>2421495</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="1">
+        <v>1019050</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>2018</v>
       </c>
       <c r="B27" s="1">
         <v>2421495</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>2019</v>
       </c>
       <c r="B28" s="1">
         <v>2588478</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>2020</v>
       </c>
       <c r="B29" s="1">
         <v>2942965</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>2021</v>
       </c>
       <c r="B30" s="1">
         <v>3117218</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>2022</v>
       </c>
       <c r="B31" s="1">
         <v>2421495</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>2023</v>
       </c>
       <c r="B32" s="1">
         <v>3242026</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>2024</v>
       </c>
       <c r="B33" s="1">
         <v>4048695</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>